<commit_message>
update package for read excel, validate import users ans hotfix actions bootstrap table
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -55,26 +55,58 @@
     <t xml:space="preserve">msalazar</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">msalazar@gmail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.com</t>
-    </r>
+    <t xml:space="preserve">msalazar@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deportes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desplazamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniuski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tizamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dtizamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dtizamo@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Física</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrición</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microbiología </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aperez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aperez@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lengua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natación  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fútbol</t>
   </si>
 </sst>
 </file>
@@ -89,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,6 +143,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,17 +214,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,12 +272,64 @@
       <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="msalazar@gmail"/>
+    <hyperlink ref="D2" r:id="rId1" display="msalazar@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="dtizamo@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="aperez@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add detailview bootstrap table, add filter with  query raw
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,24 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <si>
-    <t xml:space="preserve">first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">área</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subarea 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+  <si>
+    <t xml:space="preserve">Nombres (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apellidos (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de usuario (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correo electronico (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Área (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subarea 1 (*)</t>
   </si>
   <si>
     <t xml:space="preserve">Subarea 2</t>
@@ -46,6 +46,33 @@
     <t xml:space="preserve">Subarea 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Género (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cédula o pasaporte (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Línea de investigación (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teléfono oficina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teléfono celular o habitación (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institución donde  trabaja </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos de la institución</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observaciones</t>
+  </si>
+  <si>
     <t xml:space="preserve">María</t>
   </si>
   <si>
@@ -58,55 +85,109 @@
     <t xml:space="preserve">msalazar@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Computación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redes de computadoras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistemas de Información</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnologías de para el desarrollo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniuski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tizamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dtizamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dtizamo@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biología</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrición</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microbiología </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aperez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aperez@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Deportes</t>
   </si>
   <si>
-    <t xml:space="preserve">Velocidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desplazamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniuski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tizamo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dtizamo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dtizamo@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Física</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutrición</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microbiología </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adriana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aperez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aperez@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lengua</t>
-  </si>
-  <si>
     <t xml:space="preserve">Natación  </t>
   </si>
   <si>
     <t xml:space="preserve">Fútbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachiller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educación Física </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yohana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padrino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ypadrino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ypadrino@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño de Templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hernan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abreu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habreu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habreu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masculino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollo de aplicaciones</t>
   </si>
 </sst>
 </file>
@@ -188,8 +269,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,115 +299,269 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>20789251</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>4166542358</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>20361852</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>4127851421</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>20996361</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>4129873512</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="I5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>20798452</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>4167892530</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>28</v>
+      <c r="I6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>19526314</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>4168523678</v>
       </c>
     </row>
   </sheetData>
@@ -330,6 +569,8 @@
     <hyperlink ref="D2" r:id="rId1" display="msalazar@gmail.com"/>
     <hyperlink ref="D3" r:id="rId2" display="dtizamo@gmail.com"/>
     <hyperlink ref="D4" r:id="rId3" display="aperez@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="ypadrino@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId5" display="habreu@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
CRUD arbitros view, edit and filter search
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t xml:space="preserve">Nombres (*)</t>
   </si>
@@ -73,16 +73,61 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">María</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salazar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">msalazar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">msalazar@gmail.com</t>
+    <t xml:space="preserve">Emilia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurbina@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biociencias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parasitología</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bioquímica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genética aplicada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maurbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">murbina@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magallanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmagallanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmagallanes@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tecnología</t>
@@ -91,100 +136,10 @@
     <t xml:space="preserve">Computación</t>
   </si>
   <si>
-    <t xml:space="preserve">Ingeniería Electrónica y Biomédica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Femenino</t>
+    <t xml:space="preserve">Masculino</t>
   </si>
   <si>
     <t xml:space="preserve">Ingeniero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnologías de para el desarrollo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniuski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tizamo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dtizamo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dtizamo@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biociencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parasitología</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioquímica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licenciado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigación celular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adriana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aperez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aperez@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ciencias Exactas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matemática</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Química Organometálica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bachiller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Educación Física </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yohana </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Padrino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ypadrino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ypadrino@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diseño de Templates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hernan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abreu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habreu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habreu@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masculino</t>
   </si>
   <si>
     <t xml:space="preserve">Desarrollo de aplicaciones</t>
@@ -299,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,7 +335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>17</v>
       </c>
@@ -406,7 +361,7 @@
         <v>24</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>20789251</v>
+        <v>2074967</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>25</v>
@@ -415,7 +370,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>4166542358</v>
+        <v>4168523651</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,154 +378,79 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>20361852</v>
+        <v>45869632</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>4127851421</v>
+        <v>4168546321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="J4" s="0" t="n">
+        <v>156423651</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>20996361</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="N4" s="0" t="n">
-        <v>4129873512</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>20798452</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>4167892530</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>19526314</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>4168523678</v>
+        <v>4125658574</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="msalazar@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="dtizamo@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId3" display="aperez@gmail.com"/>
-    <hyperlink ref="D5" r:id="rId4" display="ypadrino@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId5" display="habreu@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="eurbina@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="murbina@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="jmagallanes@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
hotfix of query for jobs and select referee
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -73,49 +73,49 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
+    <t xml:space="preserve">Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maurbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">murbina@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biociencias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parasitología</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bioquímica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación celular</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emilia</t>
   </si>
   <si>
-    <t xml:space="preserve">Urbina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eurbina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eurbina@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biociencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parasitología</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioquímica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Femenino</t>
+    <t xml:space="preserve">eurbina2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurbina2@hotmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Licenciado</t>
   </si>
   <si>
     <t xml:space="preserve">Genética aplicada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maurbina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">murbina@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licenciado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigación celular</t>
   </si>
   <si>
     <t xml:space="preserve">Joan</t>
@@ -256,8 +256,8 @@
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -361,7 +361,7 @@
         <v>24</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>2074967</v>
+        <v>45869632</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>25</v>
@@ -370,7 +370,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>4168523651</v>
+        <v>4168546321</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,7 +399,7 @@
         <v>24</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>45869632</v>
+        <v>2074967</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>30</v>
@@ -408,7 +408,7 @@
         <v>31</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>4168546321</v>
+        <v>4168523651</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,8 +448,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="eurbina@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="murbina@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="murbina@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="eurbina2@hotmail"/>
     <hyperlink ref="D4" r:id="rId3" display="jmagallanes@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
user load settings and views
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">maurbina</t>
   </si>
   <si>
-    <t xml:space="preserve">murbina@gmail.com</t>
+    <t xml:space="preserve">murbina@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Biociencias</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">eurbina2</t>
   </si>
   <si>
-    <t xml:space="preserve">eurbina2@hotmail.com</t>
+    <t xml:space="preserve">eurbina@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Licenciado</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">jmagallanes</t>
   </si>
   <si>
-    <t xml:space="preserve">jmagallanes@gmail.com</t>
+    <t xml:space="preserve">jmagallanes@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tecnología</t>
@@ -257,7 +257,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -265,7 +265,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.92"/>
@@ -448,9 +448,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="murbina@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="eurbina2@hotmail"/>
-    <hyperlink ref="D4" r:id="rId3" display="jmagallanes@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="murbina@yopmail"/>
+    <hyperlink ref="D4" r:id="rId2" display="jmagallanes@yopmail"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
change constructor of FromData for upload files
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t xml:space="preserve">Nombres (*)</t>
   </si>
@@ -73,16 +73,16 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Pedro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paredes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paredesp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paredesp@yopmail.com</t>
+    <t xml:space="preserve">Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maurbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">murbina@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Biociencias</t>
@@ -94,34 +94,55 @@
     <t xml:space="preserve">Bioquímica</t>
   </si>
   <si>
+    <t xml:space="preserve">Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurbina2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurbina@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genética aplicada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magallanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmagallanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmagallanes@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnología</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computación</t>
+  </si>
+  <si>
     <t xml:space="preserve">Masculino</t>
   </si>
   <si>
-    <t xml:space="preserve">Licenciado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigación celular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mjames</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mjames@yopmail.col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Femenino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licenciado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genética aplicada</t>
+    <t xml:space="preserve">Ingeniero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollo de aplicaciones</t>
   </si>
 </sst>
 </file>
@@ -233,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -357,13 +378,13 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>21</v>
@@ -375,25 +396,60 @@
         <v>23</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>2074967</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>4168523651</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>156423651</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>4125658574</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="paredesp@yopmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="mjames@yopmail.col"/>
+    <hyperlink ref="D2" r:id="rId1" display="murbina@yopmail"/>
+    <hyperlink ref="D4" r:id="rId2" display="jmagallanes@yopmail"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update query for delete arbitro for event
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t xml:space="preserve">Nombres (*)</t>
   </si>
@@ -73,16 +73,16 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urbina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maurbina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">murbina@yopmail.com</t>
+    <t xml:space="preserve">Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paredes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paredesp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paredesp@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Biociencias</t>
@@ -94,55 +94,34 @@
     <t xml:space="preserve">Bioquímica</t>
   </si>
   <si>
+    <t xml:space="preserve">Masculino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mjames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mjames@yopmail.col</t>
+  </si>
+  <si>
     <t xml:space="preserve">Femenino</t>
   </si>
   <si>
-    <t xml:space="preserve">Licenciado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigación celular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emilia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eurbina2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eurbina@yopmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Licenciado</t>
   </si>
   <si>
     <t xml:space="preserve">Genética aplicada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magallanes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jmagallanes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jmagallanes@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnología</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masculino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingeniero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desarrollo de aplicaciones</t>
   </si>
 </sst>
 </file>
@@ -254,10 +233,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -378,13 +357,13 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>21</v>
@@ -396,60 +375,25 @@
         <v>23</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>2074967</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>4168523651</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>156423651</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>4125658574</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="murbina@yopmail"/>
-    <hyperlink ref="D4" r:id="rId2" display="jmagallanes@yopmail"/>
+    <hyperlink ref="D2" r:id="rId1" display="paredesp@yopmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="mjames@yopmail.col"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
corrections from 16 to 20
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t xml:space="preserve">Nombres (*)</t>
   </si>
@@ -31,19 +31,19 @@
     <t xml:space="preserve">Nombre de usuario (*)</t>
   </si>
   <si>
-    <t xml:space="preserve">Correo electrónico (*)</t>
+    <t xml:space="preserve">Correo electronico (*)</t>
   </si>
   <si>
     <t xml:space="preserve">Área (*)</t>
   </si>
   <si>
-    <t xml:space="preserve">Subárea 1 (*)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subárea 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subárea 3</t>
+    <t xml:space="preserve">Subarea 1 (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subarea 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subarea 3</t>
   </si>
   <si>
     <t xml:space="preserve">Género (*)</t>
@@ -73,16 +73,16 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Pedro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paredes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paredesp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paredesp@yopmail.com</t>
+    <t xml:space="preserve">Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maurbina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">murbina@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Biociencias</t>
@@ -94,34 +94,55 @@
     <t xml:space="preserve">Bioquímica</t>
   </si>
   <si>
+    <t xml:space="preserve">Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurbina2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurbina@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genética aplicada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magallanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmagallanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmagallanes@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnología</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computación</t>
+  </si>
+  <si>
     <t xml:space="preserve">Masculino</t>
   </si>
   <si>
-    <t xml:space="preserve">Licenciado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigación celular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mjames</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mjames@yopmail.col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Femenino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licenciado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genética aplicada</t>
+    <t xml:space="preserve">Ingeniero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollo de aplicaciones</t>
   </si>
 </sst>
 </file>
@@ -233,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -357,13 +378,13 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>21</v>
@@ -375,25 +396,60 @@
         <v>23</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>2074967</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>4168523651</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>156423651</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>4125658574</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="paredesp@yopmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="mjames@yopmail.col"/>
+    <hyperlink ref="D2" r:id="rId1" display="murbina@yopmail"/>
+    <hyperlink ref="D4" r:id="rId2" display="jmagallanes@yopmail"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fix permissions to author in home
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -31,19 +31,19 @@
     <t xml:space="preserve">Nombre de usuario (*)</t>
   </si>
   <si>
-    <t xml:space="preserve">Correo electronico (*)</t>
+    <t xml:space="preserve">Correo electrónico (*)</t>
   </si>
   <si>
     <t xml:space="preserve">Área (*)</t>
   </si>
   <si>
-    <t xml:space="preserve">Subarea 1 (*)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subarea 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subarea 3</t>
+    <t xml:space="preserve">Subárea 1 (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subárea 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subárea 3</t>
   </si>
   <si>
     <t xml:space="preserve">Género (*)</t>
@@ -235,8 +235,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add feedback in load_users modal
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">Nombres (*)</t>
   </si>
@@ -73,16 +73,43 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Pedro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paredes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paredesp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paredesp@yopmail.com</t>
+    <t xml:space="preserve">Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pruebas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upruebas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upruebas@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnología</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniería Electrónica y Biomédica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masculino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnologías de para el desarrollo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prueba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pusuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pusuario@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Biociencias</t>
@@ -94,34 +121,13 @@
     <t xml:space="preserve">Bioquímica</t>
   </si>
   <si>
-    <t xml:space="preserve">Masculino</t>
+    <t xml:space="preserve">Femenino</t>
   </si>
   <si>
     <t xml:space="preserve">Licenciado </t>
   </si>
   <si>
     <t xml:space="preserve">Investigación celular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mjames</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mjames@yopmail.col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Femenino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licenciado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genética aplicada</t>
   </si>
 </sst>
 </file>
@@ -235,8 +241,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -244,7 +250,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.92"/>
@@ -340,7 +346,7 @@
         <v>24</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>45869632</v>
+        <v>20786958</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>25</v>
@@ -349,7 +355,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>4168546321</v>
+        <v>4166542358</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,43 +363,42 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>2074967</v>
+        <v>20361852</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>4168523651</v>
+        <v>4127851421</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="paredesp@yopmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="mjames@yopmail.col"/>
+    <hyperlink ref="D2" r:id="rId1" display="upruebas@yopmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fix in  loar area coordinators
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaUsuarios.xlsx
+++ b/teg_asovac_src/upload/cargaUsuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t xml:space="preserve">Nombres (*)</t>
   </si>
@@ -73,61 +73,55 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pruebas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upruebas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upruebas@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnología</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingeniería Electrónica y Biomédica</t>
+    <t xml:space="preserve">Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paredes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paredesp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paredesp@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQM</t>
   </si>
   <si>
     <t xml:space="preserve">Masculino</t>
   </si>
   <si>
-    <t xml:space="preserve">Ingeniero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnologías de para el desarrollo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prueba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pusuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pusuario@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biociencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parasitología</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioquímica</t>
+    <t xml:space="preserve">Licenciado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mjames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mjames@yopmail.col</t>
   </si>
   <si>
     <t xml:space="preserve">Femenino</t>
   </si>
   <si>
-    <t xml:space="preserve">Licenciado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigación celular</t>
+    <t xml:space="preserve">Licenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genética aplicada</t>
   </si>
 </sst>
 </file>
@@ -242,7 +236,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,7 +244,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.92"/>
@@ -346,7 +340,7 @@
         <v>24</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>20786958</v>
+        <v>45869632</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>25</v>
@@ -355,7 +349,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>4166542358</v>
+        <v>4168546321</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,42 +357,43 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="0" t="n">
+        <v>2074967</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>20361852</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="N3" s="0" t="n">
-        <v>4127851421</v>
+        <v>4168523651</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="upruebas@yopmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="paredesp@yopmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="mjames@yopmail.col"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>